<commit_message>
12/21/2022 started cleaned OD by NCs
</commit_message>
<xml_diff>
--- a/data/LADOT/Summary Stats of LADOT Data.xlsx
+++ b/data/LADOT/Summary Stats of LADOT Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\APP\APP\data\LADOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DCCAA8-F506-42AC-BF85-5059E0E44AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC423589-DE55-42F0-9687-81048FFF0596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{409E4451-380E-4DAC-B544-1D8158E25F34}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="39">
   <si>
     <t>Mean</t>
   </si>
@@ -120,13 +120,46 @@
   </si>
   <si>
     <t>Avg Deployment for Westwood NC in 2022</t>
+  </si>
+  <si>
+    <t>Aug 2019 Rampart (origin) to Hollywood United (destination) has "jeffers" instead of a numeric value. Can we get this value?</t>
+  </si>
+  <si>
+    <t>Summary Tables of data from "Neighborhood Council Trip Matrix" workbooks</t>
+  </si>
+  <si>
+    <t>Total Trip Counts from "Trip Origin-Destination Neighborhood Council Districts" workbook</t>
+  </si>
+  <si>
+    <t>Venice Jan 2019</t>
+  </si>
+  <si>
+    <t>East Hollywood June 2019</t>
+  </si>
+  <si>
+    <t>United Neighborhoods of the Historic Arlington Heights for Feb 2020</t>
+  </si>
+  <si>
+    <t>Mid City West CC for July 2020</t>
+  </si>
+  <si>
+    <t>East Hollywood NC for Mar 2021</t>
+  </si>
+  <si>
+    <t>Elysian Valley Riverside NC for Aug 2021</t>
+  </si>
+  <si>
+    <t>Sherman Oaks for Apr 2022</t>
+  </si>
+  <si>
+    <t>Eagle Rock NC for Sept 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +171,27 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,23 +234,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{FC67EECA-2581-4E83-B08F-F41D3CF75E8F}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{8335DA37-AC2F-4F68-A9B8-4E6656341F74}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,1088 +562,1149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37A8C1-469A-4A28-8E10-81B6D214BF1C}">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="E2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="H2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="M1" s="5" t="s">
+      <c r="K2" s="2"/>
+      <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="P1" s="5" t="s">
+      <c r="N2" s="2"/>
+      <c r="P2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="5"/>
-      <c r="S1" s="5" t="s">
+      <c r="Q2" s="2"/>
+      <c r="S2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="T2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="5"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="W2" s="2"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>631.26666666666665</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>255.38775510204081</v>
       </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>26.448275862068964</v>
       </c>
-      <c r="J3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>229.13953488372093</v>
       </c>
-      <c r="M3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3">
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>46.866666666666667</v>
       </c>
-      <c r="P3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q3">
+      <c r="P4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>1.5154639175257731</v>
       </c>
-      <c r="S3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T3">
+      <c r="S4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>38.5</v>
       </c>
-      <c r="V3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W3">
+      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <v>13.402061855670103</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5">
         <v>503.92287070231117</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>234.89564882938129</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>14.114150268539403</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" t="s">
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <v>191.55636743529121</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M5" t="s">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="N5">
         <v>26.313822953003189</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P5" t="s">
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="Q5">
         <v>0.66840089115885015</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S5" t="s">
         <v>1</v>
       </c>
-      <c r="T4">
+      <c r="T5">
         <v>31.067301025072265</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V5" t="s">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="W5">
         <v>10.286036515907149</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
         <v>2</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>2</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
         <v>2</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
         <v>2</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
         <v>2</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>3</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
         <v>3</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>3</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
         <v>3</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
         <v>3</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="V6" t="s">
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="V7" t="s">
         <v>3</v>
       </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8">
         <v>2760.0992352641501</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>2325.348286218572</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>131.6480295669223</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>4</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>1776.4206719778874</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M8" t="s">
         <v>4</v>
       </c>
-      <c r="N7">
+      <c r="N8">
         <v>249.63484343372377</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P8" t="s">
         <v>4</v>
       </c>
-      <c r="Q7">
+      <c r="Q8">
         <v>6.5829853316173095</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S8" t="s">
         <v>4</v>
       </c>
-      <c r="T7">
+      <c r="T8">
         <v>304.3961407874873</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V8" t="s">
         <v>4</v>
       </c>
-      <c r="W7">
+      <c r="W8">
         <v>101.30571098925174</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9">
         <v>7618147.788505747</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>5407244.6522196503</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>5</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>17331.203688853246</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>5</v>
       </c>
-      <c r="K8">
+      <c r="K9">
         <v>3155670.4038303695</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>5</v>
       </c>
-      <c r="N8">
+      <c r="N9">
         <v>62317.555056179779</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P9" t="s">
         <v>5</v>
       </c>
-      <c r="Q8">
+      <c r="Q9">
         <v>43.335695876288661</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S9" t="s">
         <v>5</v>
       </c>
-      <c r="T8">
+      <c r="T9">
         <v>92657.010526315789</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V9" t="s">
         <v>5</v>
       </c>
-      <c r="W8">
+      <c r="W9">
         <v>10262.8470790378</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10">
         <v>27.725594827301009</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>97.481857860225134</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>6</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>71.526649417139993</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>6</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <v>84.663662362822947</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" t="s">
         <v>6</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>67.7127852968746</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P10" t="s">
         <v>6</v>
       </c>
-      <c r="Q9">
+      <c r="Q10">
         <v>42.468614116336653</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S10" t="s">
         <v>6</v>
       </c>
-      <c r="T9">
+      <c r="T10">
         <v>93.752651918168041</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V10" t="s">
         <v>6</v>
       </c>
-      <c r="W9">
+      <c r="W10">
         <v>83.634890577613859</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11">
         <v>5.2061396043504482</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>9.8617783588582313</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>7</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>8.1640411190078019</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>7</v>
       </c>
-      <c r="K10">
+      <c r="K11">
         <v>9.1700450588238969</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>7</v>
       </c>
-      <c r="N10">
+      <c r="N11">
         <v>7.9088002407714049</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P11" t="s">
         <v>7</v>
       </c>
-      <c r="Q10">
+      <c r="Q11">
         <v>6.1455947969402835</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S11" t="s">
         <v>7</v>
       </c>
-      <c r="T10">
+      <c r="T11">
         <v>9.6335139052921797</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V11" t="s">
         <v>7</v>
       </c>
-      <c r="W10">
+      <c r="W11">
         <v>8.9707977660192135</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12">
         <v>14987</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>23011</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>8</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>1184</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>8</v>
       </c>
-      <c r="K11">
+      <c r="K12">
         <v>16450</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>8</v>
       </c>
-      <c r="N11">
+      <c r="N12">
         <v>2230</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P12" t="s">
         <v>8</v>
       </c>
-      <c r="Q11">
+      <c r="Q12">
         <v>53</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S12" t="s">
         <v>8</v>
       </c>
-      <c r="T11">
+      <c r="T12">
         <v>2973</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V12" t="s">
         <v>8</v>
       </c>
-      <c r="W11">
+      <c r="W12">
         <v>965</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
         <v>9</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>9</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
         <v>9</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="S12" t="s">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
         <v>9</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="V12" t="s">
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="V13" t="s">
         <v>9</v>
       </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14">
         <v>14987</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>23011</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>10</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>1184</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>16450</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M14" t="s">
         <v>10</v>
       </c>
-      <c r="N13">
+      <c r="N14">
         <v>2230</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P14" t="s">
         <v>10</v>
       </c>
-      <c r="Q13">
+      <c r="Q14">
         <v>53</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S14" t="s">
         <v>10</v>
       </c>
-      <c r="T13">
+      <c r="T14">
         <v>2973</v>
       </c>
-      <c r="V13" t="s">
+      <c r="V14" t="s">
         <v>10</v>
       </c>
-      <c r="W13">
+      <c r="W14">
         <v>965</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="3">
         <v>18938</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E14">
+      <c r="E15" s="3">
         <v>25028</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H14">
+      <c r="H15" s="3">
         <v>2301</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K14">
+      <c r="K15" s="3">
         <v>19706</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N14">
+      <c r="N15" s="3">
         <v>4218</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q14">
+      <c r="Q15" s="3">
         <v>147</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T14">
+      <c r="T15" s="3">
         <v>3696</v>
       </c>
-      <c r="V14" t="s">
+      <c r="V15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="W14">
+      <c r="W15" s="3">
         <v>1300</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="1">
         <v>30</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E16" s="1">
         <v>98</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="1">
         <v>87</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K16" s="1">
         <v>86</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N16" s="1">
         <v>90</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q16" s="1">
         <v>97</v>
       </c>
-      <c r="S15" s="3" t="s">
+      <c r="S16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T16" s="1">
         <v>96</v>
       </c>
-      <c r="V15" s="3" t="s">
+      <c r="V16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W16" s="1">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>19004</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>24061</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19">
+        <v>2311</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19">
+        <v>19843</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19">
+        <v>4100</v>
+      </c>
+      <c r="P19" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q19">
+        <v>141</v>
+      </c>
+      <c r="S19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19">
+        <v>3691</v>
+      </c>
+      <c r="V19" t="s">
+        <v>38</v>
+      </c>
+      <c r="W19">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="D24" s="5" t="s">
+      <c r="B28" s="2"/>
+      <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="G24" s="5" t="s">
+      <c r="E28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="J24" s="5" t="s">
+      <c r="H28" s="2"/>
+      <c r="J28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26">
+      <c r="K28" s="2"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
         <v>172.95959595959596</v>
       </c>
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>70.878787878787875</v>
       </c>
-      <c r="G26" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26">
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>207.75</v>
       </c>
-      <c r="J26" t="s">
-        <v>0</v>
-      </c>
-      <c r="K26">
+      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30">
         <v>102.55555555555556</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>1</v>
       </c>
-      <c r="B27">
+      <c r="B31">
         <v>49.452760638559596</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D31" t="s">
         <v>1</v>
       </c>
-      <c r="E27">
+      <c r="E31">
         <v>19.71930563650961</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G31" t="s">
         <v>1</v>
       </c>
-      <c r="H27">
+      <c r="H31">
         <v>13.966477723463422</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J31" t="s">
         <v>1</v>
       </c>
-      <c r="K27">
+      <c r="K31">
         <v>2.7844364635870371</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>2</v>
       </c>
-      <c r="B28">
+      <c r="B32">
         <v>18</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D32" t="s">
         <v>2</v>
       </c>
-      <c r="E28">
+      <c r="E32">
         <v>8</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G32" t="s">
         <v>2</v>
       </c>
-      <c r="H28">
+      <c r="H32">
         <v>202.5</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J32" t="s">
         <v>2</v>
       </c>
-      <c r="K28">
+      <c r="K32">
         <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
-        <v>3</v>
-      </c>
-      <c r="H29">
-        <v>240</v>
-      </c>
-      <c r="J29" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30">
-        <v>492.04875565607546</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30">
-        <v>196.20461376792821</v>
-      </c>
-      <c r="G30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30">
-        <v>48.381298039635105</v>
-      </c>
-      <c r="J30" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30">
-        <v>8.3533093907611118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>242111.97794269223</v>
-      </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31">
-        <v>38496.250463821889</v>
-      </c>
-      <c r="G31" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31">
-        <v>2340.75</v>
-      </c>
-      <c r="J31" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31">
-        <v>69.777777777777771</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>39.445337509147876</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <v>39.305074662009503</v>
-      </c>
-      <c r="G32" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32">
-        <v>-0.53000947683053212</v>
-      </c>
-      <c r="J32" t="s">
-        <v>6</v>
-      </c>
-      <c r="K32">
-        <v>0.55073934468509211</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B33">
-        <v>5.7656134228906311</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E33">
-        <v>5.6335299909981584</v>
+        <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H33">
-        <v>0.6641718145513803</v>
+        <v>240</v>
       </c>
       <c r="J33" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K33">
-        <v>0.74531302613534633</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>3989</v>
+        <v>492.04875565607546</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>1607</v>
+        <v>196.20461376792821</v>
       </c>
       <c r="G34" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>145</v>
+        <v>48.381298039635105</v>
       </c>
       <c r="J34" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K34">
-        <v>27</v>
+        <v>8.3533093907611118</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>242111.97794269223</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>38496.250463821889</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H35">
-        <v>155</v>
+        <v>2340.75</v>
       </c>
       <c r="J35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K35">
-        <v>92</v>
+        <v>69.777777777777771</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B36">
-        <v>3989</v>
+        <v>39.445337509147876</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>1607</v>
+        <v>39.305074662009503</v>
       </c>
       <c r="G36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H36">
-        <v>300</v>
+        <v>-0.53000947683053212</v>
       </c>
       <c r="J36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K36">
-        <v>119</v>
+        <v>0.55073934468509211</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>5.7656134228906311</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>5.6335299909981584</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <v>0.6641718145513803</v>
+      </c>
+      <c r="J37" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37">
+        <v>0.74531302613534633</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>3989</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>1607</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <v>145</v>
+      </c>
+      <c r="J38" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <v>155</v>
+      </c>
+      <c r="J39" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>3989</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>1607</v>
+      </c>
+      <c r="G40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>300</v>
+      </c>
+      <c r="J40" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>11</v>
       </c>
-      <c r="B37">
+      <c r="B41">
         <v>17123</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="E37">
+      <c r="E41">
         <v>7017</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G41" t="s">
         <v>11</v>
       </c>
-      <c r="H37">
+      <c r="H41">
         <v>2493</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J41" t="s">
         <v>11</v>
       </c>
-      <c r="K37">
+      <c r="K41">
         <v>923</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="3" t="s">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B42" s="1">
         <v>99</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E42" s="1">
         <v>99</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H42" s="1">
         <v>12</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K42" s="1">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>